<commit_message>
Added faulty disconnect data and used most recent charger data
</commit_message>
<xml_diff>
--- a/Chargerlocations.xlsx
+++ b/Chargerlocations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgutierrez.MYSMITHFIELD\PycharmProjects\Chargerdataprocessor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A294822-30CE-49E5-ACE4-3DD19B72B6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828DC97E-5C8B-4331-9D5E-190D066FAA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22440" yWindow="-330" windowWidth="14100" windowHeight="10710" xr2:uid="{5F318202-7931-4863-97A9-CC32D701A797}"/>
+    <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{5F318202-7931-4863-97A9-CC32D701A797}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="In Use" sheetId="1" r:id="rId1"/>
+    <sheet name="Not In Use" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>Location</t>
   </si>
@@ -123,21 +124,6 @@
     <t>Cooler 2</t>
   </si>
   <si>
-    <t>CA-1</t>
-  </si>
-  <si>
-    <t>CA-2</t>
-  </si>
-  <si>
-    <t>CA-3</t>
-  </si>
-  <si>
-    <t>DS-1</t>
-  </si>
-  <si>
-    <t>DS-2</t>
-  </si>
-  <si>
     <t>OR-1</t>
   </si>
   <si>
@@ -159,9 +145,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Enersys mods</t>
-  </si>
-  <si>
     <t>ML195059</t>
   </si>
   <si>
@@ -201,10 +184,64 @@
     <t>Oldie</t>
   </si>
   <si>
-    <t>HF23</t>
-  </si>
-  <si>
-    <t>IQ9</t>
+    <t>Spare mods</t>
+  </si>
+  <si>
+    <t>CPR1</t>
+  </si>
+  <si>
+    <t>CPR2</t>
+  </si>
+  <si>
+    <t>HFIQ 9</t>
+  </si>
+  <si>
+    <t>HF 23</t>
+  </si>
+  <si>
+    <t>FAULTED</t>
+  </si>
+  <si>
+    <t>Pallet</t>
+  </si>
+  <si>
+    <t>MJ190511</t>
+  </si>
+  <si>
+    <t>MJ190515</t>
+  </si>
+  <si>
+    <t>MJ190513</t>
+  </si>
+  <si>
+    <t>MJ190516</t>
+  </si>
+  <si>
+    <t>PI504327</t>
+  </si>
+  <si>
+    <t>PI504324</t>
+  </si>
+  <si>
+    <t>PI504326</t>
+  </si>
+  <si>
+    <t>CA1</t>
+  </si>
+  <si>
+    <t>CA2</t>
+  </si>
+  <si>
+    <t>CA3</t>
+  </si>
+  <si>
+    <t>MJ190504</t>
+  </si>
+  <si>
+    <t>unplugged</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -563,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE12825-5FA0-48A1-B0CB-3F43941314C4}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,6 +611,346 @@
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B54BEA4-CAAD-461C-8F8F-E2109E12ECE9}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -587,312 +964,107 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>